<commit_message>
se re estructura la tabla de la vista
</commit_message>
<xml_diff>
--- a/assets/archivos/archivoExcel.xlsx
+++ b/assets/archivos/archivoExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SIANDSI 4\Desktop\Trabajos UCC\Mexico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7222512-2767-46E5-A6BC-10355F356FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6CB068-6D9D-400E-A754-D804557BF942}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -933,10 +933,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1235,32 +1235,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="A6" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1759,7 +1759,7 @@
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1893,9 +1893,9 @@
         <v>1</v>
       </c>
       <c r="C2" s="24">
-        <v>21</v>
-      </c>
-      <c r="D2" s="32">
+        <v>20</v>
+      </c>
+      <c r="D2" s="31">
         <v>44177</v>
       </c>
       <c r="E2" s="24" t="s">
@@ -1987,7 +1987,7 @@
       <c r="C3" s="30">
         <v>2</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="31">
         <v>44178</v>
       </c>
       <c r="E3" s="30" t="s">
@@ -2079,7 +2079,7 @@
       <c r="C4" s="30">
         <v>2</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <v>44179</v>
       </c>
       <c r="E4" s="30" t="s">

</xml_diff>

<commit_message>
se realiza creacion de excel con errores marcados en casillas
</commit_message>
<xml_diff>
--- a/assets/archivos/archivoExcel.xlsx
+++ b/assets/archivos/archivoExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SIANDSI 4\Desktop\Trabajos UCC\Mexico\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SIANDSI 4\Desktop\Trabajos UCC\Mexico\Trabajo 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6CB068-6D9D-400E-A754-D804557BF942}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AAFE8F-096B-4ED1-9CFC-28D21C84691B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="217">
   <si>
     <t>ARCHIVOS QUINCENALES</t>
   </si>
@@ -675,6 +675,9 @@
   </si>
   <si>
     <t>aa</t>
+  </si>
+  <si>
+    <t>VEBR771220MJCLRQ01</t>
   </si>
 </sst>
 </file>
@@ -1759,7 +1762,7 @@
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,7 +1774,8 @@
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
@@ -2095,7 +2099,7 @@
         <v>66</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>67</v>
+        <v>216</v>
       </c>
       <c r="J4" s="30">
         <v>123456789121212</v>

</xml_diff>